<commit_message>
uploaded a few visualizations from the excel files
</commit_message>
<xml_diff>
--- a/2.11.Covariance-exercise.xlsx
+++ b/2.11.Covariance-exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Downloads/The Data Science Course 2021 - All Resources/Part_3_Statistics/S15_L90/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Desktop/Excel Work/365-Data-Science-Course-Excel-Work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EAF023-2A29-4044-95D8-7B56634E78F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A29A71D-A7EC-8847-B9EF-E6BF1D12BD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Covariance" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Housing data</t>
   </si>
@@ -113,7 +113,13 @@
     <t>COVARIANCE</t>
   </si>
   <si>
-    <t xml:space="preserve">There seems to be a noticeeable relationship between the variables, namely a positive relationship where the variables move in the same direction. This is evidenced by the positive covariance of 310,686 </t>
+    <t xml:space="preserve">There seems to be a noticeeable relationship between the variables, </t>
+  </si>
+  <si>
+    <t>namely a positive relationship where the variables move in the same direction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> This is evidenced by the positive covariance of 310,686 </t>
   </si>
 </sst>
 </file>
@@ -2328,9 +2334,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2368,7 +2374,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2474,7 +2480,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2616,7 +2622,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2625,10 +2631,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B1:Q22"/>
+  <dimension ref="B1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2645,20 +2651,20 @@
     <col min="13" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
@@ -2666,7 +2672,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
@@ -2677,7 +2683,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
@@ -2685,7 +2691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
@@ -2693,16 +2699,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B9" s="5"/>
-      <c r="Q9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.15">
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
@@ -2714,7 +2717,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.15">
       <c r="C12" s="16">
         <v>344</v>
       </c>
@@ -2728,7 +2731,7 @@
       <c r="J12" s="5"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.15">
       <c r="C13" s="16">
         <v>383</v>
       </c>
@@ -2741,7 +2744,7 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.15">
       <c r="C14" s="16">
         <v>611</v>
       </c>
@@ -2753,7 +2756,7 @@
         <v>1179.3600000000024</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.15">
       <c r="C15" s="16">
         <v>713</v>
       </c>
@@ -2765,7 +2768,7 @@
         <v>44714.160000000011</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.15">
       <c r="C16" s="17">
         <v>536</v>
       </c>
@@ -2826,6 +2829,21 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.15">
       <c r="F22" s="5"/>
       <c r="G22" s="9"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C27" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G12:G20">

</xml_diff>